<commit_message>
Modulo Overflow bug fixed
</commit_message>
<xml_diff>
--- a/3_Unterprogramme/stepper/motorCalc.xlsx
+++ b/3_Unterprogramme/stepper/motorCalc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janbantle/Documents/GitHub/Studienarbeit/3_Unterprogramme/stepper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47E30A15-4E51-A145-8B3A-DFC89B2D3FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA87071F-D744-FF48-8A40-5D41AEA3B7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{0CBBFBA9-D9BF-AA46-8AC4-34933E3411A4}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="8740" xr2:uid="{0CBBFBA9-D9BF-AA46-8AC4-34933E3411A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Berechnung Timer Clock --&gt; Motor Frequency </t>
   </si>
@@ -58,9 +58,6 @@
     <t xml:space="preserve">max-freq </t>
   </si>
   <si>
-    <t xml:space="preserve">1000Hz </t>
-  </si>
-  <si>
     <t>&gt; max OCR1=990</t>
   </si>
   <si>
@@ -68,6 +65,21 @@
   </si>
   <si>
     <t>&gt; min OCR1=5500</t>
+  </si>
+  <si>
+    <t>modulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeit bis k overflow: </t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>&gt; unsigned long ausreichend!</t>
   </si>
 </sst>
 </file>
@@ -421,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D917E73-4304-3642-BE3A-C32420CA985C}">
-  <dimension ref="A2:E14"/>
+  <dimension ref="A2:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="185" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -487,26 +499,1369 @@
         <v>2</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2147000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <f>B10/B13</f>
+        <v>2147000</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f>A11/3600</f>
+        <v>596.38888888888891</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13">
+        <v>1000</v>
+      </c>
+      <c r="C13" t="s">
         <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>180</v>
       </c>
       <c r="C14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>10</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <f>MOD(A19,4)</f>
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <f>MOD(A19,10)</f>
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f>MOD(A19,$D$18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B83" si="0">MOD(A20,4)</f>
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:C83" si="1">MOD(A20,10)</f>
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:D83" si="2">MOD(A20,$D$18)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>13</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>16</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>19</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>21</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>22</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>23</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>24</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>26</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>27</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>28</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>29</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>30</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>31</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>32</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>33</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>34</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>35</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>36</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>37</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>38</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>39</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>40</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>41</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>42</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>43</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>44</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>45</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>46</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>47</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>48</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>49</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>50</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>51</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>52</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>53</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>54</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>55</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>56</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>57</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>58</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>59</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>60</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>61</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>62</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>63</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>64</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>65</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>66</v>
+      </c>
+      <c r="B84">
+        <f t="shared" ref="B84:B86" si="3">MOD(A84,4)</f>
+        <v>2</v>
+      </c>
+      <c r="C84">
+        <f t="shared" ref="C84:C96" si="4">MOD(A84,10)</f>
+        <v>6</v>
+      </c>
+      <c r="D84">
+        <f t="shared" ref="D84:D97" si="5">MOD(A84,$D$18)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>67</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>68</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>69</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>70</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>71</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>72</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>73</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>74</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>75</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>76</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>77</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>78</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>79</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>